<commit_message>
20191024 - Update selectors - Microspot
</commit_message>
<xml_diff>
--- a/Data/Output/PriceComparison.xlsx
+++ b/Data/Output/PriceComparison.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="0" windowWidth="8130" windowHeight="6780"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20700" windowHeight="12345"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="45">
   <si>
     <t>Name</t>
   </si>
@@ -44,85 +44,79 @@
     <t>Price Difference</t>
   </si>
   <si>
+    <t>APPLE iPhone 11 - Smartphone (6.1 ", 128 GB, Black)</t>
+  </si>
+  <si>
+    <t>/fr/product/_apple-iphone-11-1948087.html</t>
+  </si>
+  <si>
     <t>128 GB</t>
   </si>
   <si>
+    <t>APPLE iPhone 11 - Smartphone (6.1 ", 64 GB, Black)</t>
+  </si>
+  <si>
+    <t>/fr/product/_apple-iphone-11-1948078.html</t>
+  </si>
+  <si>
     <t>64 GB</t>
   </si>
   <si>
+    <t>APPLE iPhone 11 - Smartphone (6.1 ", 128 GB, White)</t>
+  </si>
+  <si>
+    <t>/fr/product/_apple-iphone-11-1948088.html</t>
+  </si>
+  <si>
+    <t>APPLE iPhone 11 - Smartphone (6.1 ", 64 GB, White)</t>
+  </si>
+  <si>
+    <t>/fr/product/_apple-iphone-11-1948079.html</t>
+  </si>
+  <si>
+    <t>APPLE iPhone 11 - Smartphone (6.1 ", 128 GB, Purple)</t>
+  </si>
+  <si>
+    <t>/fr/product/_apple-iphone-11-1948093.html</t>
+  </si>
+  <si>
+    <t>APPLE iPhone 11 - Smartphone (6.1 ", 128 GB, Red™)</t>
+  </si>
+  <si>
+    <t>/fr/product/_apple-iphone-11-1948089.html</t>
+  </si>
+  <si>
+    <t>APPLE iPhone 11 - Smartphone (6.1 ", 64 GB, Purple)</t>
+  </si>
+  <si>
+    <t>/fr/product/_apple-iphone-11-1948085.html</t>
+  </si>
+  <si>
+    <t>APPLE iPhone 11 - Smartphone (6.1 ", 64 GB, Green)</t>
+  </si>
+  <si>
+    <t>/fr/product/_apple-iphone-11-1948086.html</t>
+  </si>
+  <si>
+    <t>APPLE iPhone 11 - Smartphone (6.1 ", 256 GB, Black)</t>
+  </si>
+  <si>
+    <t>/fr/product/_apple-iphone-11-1948096.html</t>
+  </si>
+  <si>
     <t>256 GB</t>
   </si>
   <si>
-    <t>APPLE iPhone 11 - Smartphone (6.1 ", 128 GB, Red™)</t>
-  </si>
-  <si>
-    <t>/fr/product/_apple-iphone-11-1948089.html</t>
-  </si>
-  <si>
-    <t>APPLE iPhone 11 - Smartphone (6.1 ", 128 GB, Black)</t>
-  </si>
-  <si>
-    <t>/fr/product/_apple-iphone-11-1948087.html</t>
-  </si>
-  <si>
-    <t>APPLE iPhone 11 - Smartphone (6.1 ", 256 GB, Black)</t>
-  </si>
-  <si>
-    <t>/fr/product/_apple-iphone-11-1948096.html</t>
-  </si>
-  <si>
-    <t>APPLE iPhone 11 - Smartphone (6.1 ", 128 GB, Purple)</t>
-  </si>
-  <si>
-    <t>/fr/product/_apple-iphone-11-1948093.html</t>
-  </si>
-  <si>
-    <t>APPLE iPhone 11 - Smartphone (6.1 ", 64 GB, Green)</t>
-  </si>
-  <si>
-    <t>/fr/product/_apple-iphone-11-1948086.html</t>
-  </si>
-  <si>
-    <t>APPLE iPhone 11 Pro - Smartphone (5.8 ", 256 GB, Midnight Green)</t>
-  </si>
-  <si>
-    <t>/fr/product/_apple-iphone-11-pro-1948118.html</t>
-  </si>
-  <si>
-    <t>APPLE iPhone 11 - Smartphone (6.1 ", 128 GB, White)</t>
-  </si>
-  <si>
-    <t>/fr/product/_apple-iphone-11-1948088.html</t>
-  </si>
-  <si>
-    <t>APPLE iPhone 11 - Smartphone (6.1 ", 64 GB, Black)</t>
-  </si>
-  <si>
-    <t>/fr/product/_apple-iphone-11-1948078.html</t>
-  </si>
-  <si>
-    <t>APPLE iPhone 11 Pro - Smartphone (5.8 ", 256 GB, Space Grey)</t>
-  </si>
-  <si>
-    <t>/fr/product/_apple-iphone-11-pro-1948113.html</t>
-  </si>
-  <si>
-    <t>APPLE iPhone 11 Pro - Smartphone (5.8 ", 64 GB, Midnight Green)</t>
-  </si>
-  <si>
-    <t>/fr/product/_apple-iphone-11-pro-1948111.html</t>
-  </si>
-  <si>
     <t>APPLE iPhone 11 - Smartphone (6.1 ", 64 GB, Red™)</t>
   </si>
   <si>
     <t>/fr/product/_apple-iphone-11-1948082.html</t>
   </si>
   <si>
-    <t>APPLE iPhone 11 Pro - Smartphone (5.8 ", 64 GB, Space Grey)</t>
-  </si>
-  <si>
-    <t>/fr/product/_apple-iphone-11-pro-1948106.html</t>
+    <t>APPLE iPhone 11 - Smartphone (6.1 ", 128 GB, Green)</t>
+  </si>
+  <si>
+    <t>/fr/product/_apple-iphone-11-1948094.html</t>
   </si>
   <si>
     <t>APPLE iPhone 11 - Smartphone (6.1 ", 64 GB, Yellow)</t>
@@ -131,67 +125,16 @@
     <t>/fr/product/_apple-iphone-11-1948084.html</t>
   </si>
   <si>
-    <t>APPLE iPhone 11 - Smartphone (6.1 ", 64 GB, Purple)</t>
-  </si>
-  <si>
-    <t>/fr/product/_apple-iphone-11-1948085.html</t>
-  </si>
-  <si>
-    <t>APPLE iPhone 11 Pro Max - Smartphone (6.5 ", 64 GB, Space Grey)</t>
-  </si>
-  <si>
-    <t>/fr/product/_apple-iphone-11-pro-max-1948123.html</t>
-  </si>
-  <si>
-    <t>APPLE iPhone 11 - Smartphone (6.1 ", 128 GB, Green)</t>
-  </si>
-  <si>
-    <t>/fr/product/_apple-iphone-11-1948094.html</t>
-  </si>
-  <si>
-    <t>APPLE iPhone 11 Pro Max - Smartphone (6.5 ", 64 GB, Midnight Green)</t>
-  </si>
-  <si>
-    <t>/fr/product/_apple-iphone-11-pro-max-1948127.html</t>
-  </si>
-  <si>
-    <t>APPLE iPhone 11 Pro Max - Smartphone (6.5 ", 256 GB, Gold)</t>
-  </si>
-  <si>
-    <t>/fr/product/_apple-iphone-11-pro-max-1948132.html</t>
-  </si>
-  <si>
-    <t>APPLE iPhone 11 - Smartphone (6.1 ", 64 GB, White)</t>
-  </si>
-  <si>
-    <t>/fr/product/_apple-iphone-11-1948079.html</t>
-  </si>
-  <si>
-    <t>APPLE iPhone 11 Pro - Smartphone (5.8 ", 64 GB, Silver)</t>
-  </si>
-  <si>
-    <t>/fr/product/_apple-iphone-11-pro-1948107.html</t>
-  </si>
-  <si>
-    <t>APPLE iPhone 11 Pro - Smartphone (5.8 ", 256 GB, Gold)</t>
-  </si>
-  <si>
-    <t>/fr/product/_apple-iphone-11-pro-1948117.html</t>
-  </si>
-  <si>
-    <t>APPLE iPhone 11 Pro Max - Smartphone (6.5 ", 256 GB, Silver)</t>
-  </si>
-  <si>
-    <t>/fr/product/_apple-iphone-11-pro-max-1948130.html</t>
-  </si>
-  <si>
-    <t>APPLE iPhone 11 Pro - Smartphone (5.8 ", 512 GB, Midnight Green)</t>
-  </si>
-  <si>
-    <t>/fr/product/_apple-iphone-11-pro-1948122.html</t>
-  </si>
-  <si>
-    <t>512 GB</t>
+    <t>APPLE iPhone 11 - Smartphone (6.1 ", 256 GB, Purple)</t>
+  </si>
+  <si>
+    <t>/fr/product/_apple-iphone-11-1948102.html</t>
+  </si>
+  <si>
+    <t>APPLE iPhone 11 - Smartphone (6.1 ", 256 GB, White)</t>
+  </si>
+  <si>
+    <t>/fr/product/_apple-iphone-11-1948097.html</t>
   </si>
   <si>
     <t>APPLE iPhone 11 - Smartphone (6.1 ", 128 GB, Yellow)</t>
@@ -200,10 +143,22 @@
     <t>/fr/product/_apple-iphone-11-1948091.html</t>
   </si>
   <si>
-    <t>APPLE iPhone 11 Pro - Smartphone (5.8 ", 256 GB, Silver)</t>
-  </si>
-  <si>
-    <t>/fr/product/_apple-iphone-11-pro-1948115.html</t>
+    <t>APPLE iPhone 11 - Smartphone (6.1 ", 256 GB, Yellow)</t>
+  </si>
+  <si>
+    <t>/fr/product/_apple-iphone-11-1948100.html</t>
+  </si>
+  <si>
+    <t>APPLE iPhone 11 - Smartphone (6.1 ", 256 GB, Green)</t>
+  </si>
+  <si>
+    <t>/fr/product/_apple-iphone-11-1948104.html</t>
+  </si>
+  <si>
+    <t>APPLE iPhone 11 - Smartphone (6.1 ", 256 GB, Red™)</t>
+  </si>
+  <si>
+    <t>/fr/product/_apple-iphone-11-1948098.html</t>
   </si>
 </sst>
 </file>
@@ -521,7 +476,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -549,13 +504,13 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D2">
         <v>879</v>
@@ -563,39 +518,39 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D3">
-        <v>879</v>
+        <v>809</v>
       </c>
       <c r="E3">
-        <v>878</v>
+        <v>798</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
         <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
       </c>
       <c r="D4">
-        <v>999</v>
+        <v>879</v>
       </c>
       <c r="E4">
-        <v>998</v>
+        <v>878</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -603,39 +558,39 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D5">
-        <v>879</v>
+        <v>809</v>
       </c>
       <c r="E5">
-        <v>878</v>
+        <v>798</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
         <v>17</v>
       </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D6">
-        <v>809</v>
+        <v>879</v>
       </c>
       <c r="E6">
-        <v>808</v>
+        <v>878</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -643,19 +598,19 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
         <v>19</v>
-      </c>
-      <c r="B7" t="s">
-        <v>20</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
       </c>
       <c r="D7">
-        <v>1389</v>
+        <v>879</v>
       </c>
       <c r="E7">
-        <v>1388</v>
+        <v>878</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -663,62 +618,62 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
         <v>21</v>
       </c>
-      <c r="B8" t="s">
-        <v>22</v>
-      </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D8">
-        <v>879</v>
+        <v>809</v>
       </c>
       <c r="E8">
-        <v>878</v>
+        <v>798</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
         <v>23</v>
       </c>
-      <c r="B9" t="s">
-        <v>24</v>
-      </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D9">
         <v>809</v>
       </c>
       <c r="E9">
-        <v>808</v>
+        <v>798</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
         <v>25</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>26</v>
       </c>
-      <c r="C10" t="s">
-        <v>8</v>
-      </c>
       <c r="D10">
-        <v>1389</v>
+        <v>999</v>
       </c>
       <c r="E10">
-        <v>1349</v>
+        <v>998</v>
       </c>
       <c r="F10">
-        <v>40</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -729,16 +684,16 @@
         <v>28</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D11">
-        <v>1199</v>
+        <v>809</v>
       </c>
       <c r="E11">
-        <v>1198</v>
+        <v>798</v>
       </c>
       <c r="F11">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -749,13 +704,13 @@
         <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D12">
-        <v>809</v>
+        <v>879</v>
       </c>
       <c r="E12">
-        <v>808</v>
+        <v>878</v>
       </c>
       <c r="F12">
         <v>1</v>
@@ -769,16 +724,16 @@
         <v>32</v>
       </c>
       <c r="C13" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D13">
-        <v>1199</v>
+        <v>809</v>
       </c>
       <c r="E13">
-        <v>1198</v>
+        <v>798</v>
       </c>
       <c r="F13">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -789,13 +744,13 @@
         <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="D14">
-        <v>809</v>
+        <v>999</v>
       </c>
       <c r="E14">
-        <v>808</v>
+        <v>998</v>
       </c>
       <c r="F14">
         <v>1</v>
@@ -809,13 +764,13 @@
         <v>36</v>
       </c>
       <c r="C15" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="D15">
-        <v>809</v>
+        <v>999</v>
       </c>
       <c r="E15">
-        <v>808</v>
+        <v>998</v>
       </c>
       <c r="F15">
         <v>1</v>
@@ -829,13 +784,13 @@
         <v>38</v>
       </c>
       <c r="C16" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D16">
-        <v>1299</v>
+        <v>879</v>
       </c>
       <c r="E16">
-        <v>1298</v>
+        <v>878</v>
       </c>
       <c r="F16">
         <v>1</v>
@@ -849,13 +804,13 @@
         <v>40</v>
       </c>
       <c r="C17" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="D17">
-        <v>879</v>
+        <v>999</v>
       </c>
       <c r="E17">
-        <v>878</v>
+        <v>998</v>
       </c>
       <c r="F17">
         <v>1</v>
@@ -869,13 +824,13 @@
         <v>42</v>
       </c>
       <c r="C18" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="D18">
-        <v>1299</v>
+        <v>999</v>
       </c>
       <c r="E18">
-        <v>1298</v>
+        <v>998</v>
       </c>
       <c r="F18">
         <v>1</v>
@@ -889,155 +844,15 @@
         <v>44</v>
       </c>
       <c r="C19" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="D19">
-        <v>1489</v>
+        <v>999</v>
       </c>
       <c r="E19">
-        <v>1488</v>
+        <v>998</v>
       </c>
       <c r="F19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>45</v>
-      </c>
-      <c r="B20" t="s">
-        <v>46</v>
-      </c>
-      <c r="C20" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20">
-        <v>809</v>
-      </c>
-      <c r="E20">
-        <v>808</v>
-      </c>
-      <c r="F20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>47</v>
-      </c>
-      <c r="B21" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21" t="s">
-        <v>7</v>
-      </c>
-      <c r="D21">
-        <v>1199</v>
-      </c>
-      <c r="E21">
-        <v>1198</v>
-      </c>
-      <c r="F21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>49</v>
-      </c>
-      <c r="B22" t="s">
-        <v>50</v>
-      </c>
-      <c r="C22" t="s">
-        <v>8</v>
-      </c>
-      <c r="D22">
-        <v>1389</v>
-      </c>
-      <c r="E22">
-        <v>1388</v>
-      </c>
-      <c r="F22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>51</v>
-      </c>
-      <c r="B23" t="s">
-        <v>52</v>
-      </c>
-      <c r="C23" t="s">
-        <v>8</v>
-      </c>
-      <c r="D23">
-        <v>1489</v>
-      </c>
-      <c r="E23">
-        <v>1488</v>
-      </c>
-      <c r="F23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>53</v>
-      </c>
-      <c r="B24" t="s">
-        <v>54</v>
-      </c>
-      <c r="C24" t="s">
-        <v>55</v>
-      </c>
-      <c r="D24">
-        <v>1619</v>
-      </c>
-      <c r="E24">
-        <v>1618</v>
-      </c>
-      <c r="F24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>56</v>
-      </c>
-      <c r="B25" t="s">
-        <v>57</v>
-      </c>
-      <c r="C25" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25">
-        <v>879</v>
-      </c>
-      <c r="E25">
-        <v>878</v>
-      </c>
-      <c r="F25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>58</v>
-      </c>
-      <c r="B26" t="s">
-        <v>59</v>
-      </c>
-      <c r="C26" t="s">
-        <v>8</v>
-      </c>
-      <c r="D26">
-        <v>1389</v>
-      </c>
-      <c r="E26">
-        <v>1388</v>
-      </c>
-      <c r="F26">
         <v>1</v>
       </c>
     </row>

</xml_diff>